<commit_message>
Pay Period Report in good Shape
</commit_message>
<xml_diff>
--- a/orion.web/docs/PayPeriodReport.xlsx
+++ b/orion.web/docs/PayPeriodReport.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion-web\orion.web\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2C9312-4BD2-41C3-BE72-7A9025F0885E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633DE189-7C3E-4C7E-AA56-4C6782A65308}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="PayPeriodReport" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -192,13 +192,67 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -207,9 +261,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -220,16 +272,12 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -239,13 +287,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -255,73 +303,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -330,52 +318,52 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,7 +682,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,150 +696,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="17" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="10" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -875,7 +863,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>
@@ -895,6 +882,7 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
remove Excused with and w/o pay in PP report
</commit_message>
<xml_diff>
--- a/orion.web/docs/PayPeriodReport.xlsx
+++ b/orion.web/docs/PayPeriodReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion-web\orion.web\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion\orion-web\orion.web\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328BF8F4-F9DA-4C46-A56E-C55FF0444848}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEE672A-43D7-4F4F-A414-C225CF187B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="PayPeriodReport" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Employee Information</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Holiday Hours</t>
   </si>
   <si>
-    <t>Excused w/o Pay</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>PTO</t>
-  </si>
-  <si>
-    <t>Excused w/ Pay</t>
   </si>
 </sst>
 </file>
@@ -134,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -273,19 +267,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -334,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -346,10 +327,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,9 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,22 +678,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5136E350-F41C-493E-9E21-2323FDA5FA0F}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I8"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -727,78 +705,64 @@
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -806,10 +770,8 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="20" t="s">
@@ -819,14 +781,12 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3</v>
@@ -834,12 +794,10 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -847,49 +805,43 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A5:I5"/>
+  <mergeCells count="14">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "remove Excused with and w/o pay in PP report"
This reverts commit 125bf1917375c43051cae738b8d6a30e6a18bc0b.
</commit_message>
<xml_diff>
--- a/orion.web/docs/PayPeriodReport.xlsx
+++ b/orion.web/docs/PayPeriodReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion\orion-web\orion.web\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion-web\orion.web\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEE672A-43D7-4F4F-A414-C225CF187B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328BF8F4-F9DA-4C46-A56E-C55FF0444848}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="PayPeriodReport" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Employee Information</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Holiday Hours</t>
   </si>
   <si>
+    <t>Excused w/o Pay</t>
+  </si>
+  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
   </si>
   <si>
     <t>PTO</t>
+  </si>
+  <si>
+    <t>Excused w/ Pay</t>
   </si>
 </sst>
 </file>
@@ -128,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -267,6 +273,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -315,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -327,10 +346,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,6 +382,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,22 +700,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5136E350-F41C-493E-9E21-2323FDA5FA0F}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I7" sqref="I7:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -705,64 +727,78 @@
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="22"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -770,8 +806,10 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="20" t="s">
@@ -781,12 +819,14 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3</v>
@@ -794,10 +834,12 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -805,43 +847,49 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
+  <mergeCells count="18">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A5:I5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
update PP Report grand total off by one column metadata off by two rows
</commit_message>
<xml_diff>
--- a/orion.web/docs/PayPeriodReport.xlsx
+++ b/orion.web/docs/PayPeriodReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion-web\orion.web\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion\orion-web\orion.web\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328BF8F4-F9DA-4C46-A56E-C55FF0444848}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BB1723-3697-4691-B824-47AACD9F1C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E3321AD-090E-49BA-A520-2754341A4AF1}"/>
   </bookViews>
   <sheets>
     <sheet name="PayPeriodReport" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Employee Information</t>
   </si>
@@ -61,18 +61,6 @@
   </si>
   <si>
     <t>GRAND TOTAL</t>
-  </si>
-  <si>
-    <t>Company: Orion Engineering Co., Inc</t>
-  </si>
-  <si>
-    <t>Frequency: Biweekly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reporting Period: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generated On: </t>
   </si>
   <si>
     <t>Exempt</t>
@@ -700,22 +688,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5136E350-F41C-493E-9E21-2323FDA5FA0F}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I8"/>
+      <selection activeCell="A11" sqref="A11:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -727,13 +715,13 @@
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>5</v>
@@ -742,11 +730,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -757,7 +745,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
@@ -770,7 +758,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -783,7 +771,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
@@ -796,7 +784,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -809,7 +797,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="20" t="s">
@@ -822,11 +810,11 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>3</v>
@@ -837,7 +825,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -850,33 +838,8 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A5:I5"/>
@@ -890,6 +853,11 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>